<commit_message>
mv ETROC0_QInj.ipynb to ETROC0_QInj_DGDP.ipynb
</commit_message>
<xml_diff>
--- a/leading_edge_jitter_low_pwr.xlsx
+++ b/leading_edge_jitter_low_pwr.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="102" documentId="11_F25DC773A252ABEACE02ECEE6B9863F45BDE58A1" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{390CCF82-4FA1-43D5-A4A6-74DA52103FE0}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="11_F25DC773A252ABEACE02ECEE6B9863F45BDE58A1" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{E6AA304B-9174-4331-AA33-7D0FF3DCAB8A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-9948" yWindow="-13068" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sim" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="cdet-3.4p_c1-1p-1VPA" sheetId="5" r:id="rId5"/>
     <sheet name="cdet-3.4p_c1-10f-1p2VPA" sheetId="6" r:id="rId6"/>
     <sheet name="cdet-3.4p_c1-10f-1p2VPA_202006" sheetId="7" r:id="rId7"/>
+    <sheet name="cdet-3.4p_c1-10f-1p2VPA_202007" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="13">
   <si>
     <t>ff_x</t>
   </si>
@@ -2915,8 +2916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E659110F-306A-4C9B-A24D-7C7A49E44953}">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="A1:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3345,4 +3346,437 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F784C4-A1C9-40C2-8A1A-7149482F5E61}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>4.0000000000000003E-15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3.9169986480591901E-11</v>
+      </c>
+      <c r="C2" s="1">
+        <v>4.0000000000000003E-15</v>
+      </c>
+      <c r="D2" s="1">
+        <v>4.11171214297567E-11</v>
+      </c>
+      <c r="E2" s="1">
+        <v>4.0000000000000003E-15</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3.2537806243192397E-11</v>
+      </c>
+      <c r="G2" s="1">
+        <v>4.0000000000000003E-15</v>
+      </c>
+      <c r="H2" s="1">
+        <v>3.7465408350088697E-11</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4.0000000000000003E-15</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3.5018622894719998E-11</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2.7</v>
+      </c>
+      <c r="L2" s="1">
+        <v>55.081312393576702</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>5E-15</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.6556261632019499E-11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>5E-15</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2.9358843650019399E-11</v>
+      </c>
+      <c r="E3" s="1">
+        <v>5E-15</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.5870070750583499E-11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>5E-15</v>
+      </c>
+      <c r="H3" s="1">
+        <v>3.04412323826729E-11</v>
+      </c>
+      <c r="I3" s="1">
+        <v>5E-15</v>
+      </c>
+      <c r="J3" s="1">
+        <v>2.69230441851541E-11</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="L3" s="1">
+        <v>33.596540000416098</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>5.9999999999999997E-15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2.08179813289464E-11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.9999999999999997E-15</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2.3770171819924301E-11</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.9999999999999997E-15</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2.2045360643927101E-11</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5.9999999999999997E-15</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.6507644565622301E-11</v>
+      </c>
+      <c r="I4" s="1">
+        <v>5.9999999999999997E-15</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2.2529205093820501E-11</v>
+      </c>
+      <c r="K4" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L4" s="1">
+        <v>26.053742533458099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>8.0000000000000006E-15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1.5269015418162799E-11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>8.0000000000000006E-15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.8215909402197599E-11</v>
+      </c>
+      <c r="E5" s="1">
+        <v>8.0000000000000006E-15</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1.7854374851950801E-11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>8.0000000000000006E-15</v>
+      </c>
+      <c r="H5" s="1">
+        <v>2.2301062802302001E-11</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8.0000000000000006E-15</v>
+      </c>
+      <c r="J5" s="1">
+        <v>1.78172376477341E-11</v>
+      </c>
+      <c r="K5" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="L5" s="1">
+        <v>22.5273605866244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>1E-14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.25769109690672E-11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1E-14</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.5437641152124E-11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1E-14</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1.56700729168512E-11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1E-14</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.01131494108444E-11</v>
+      </c>
+      <c r="I6" s="1">
+        <v>1E-14</v>
+      </c>
+      <c r="J6" s="1">
+        <v>1.5390808798004E-11</v>
+      </c>
+      <c r="K6" s="1">
+        <v>7.4</v>
+      </c>
+      <c r="L6" s="1">
+        <v>18.815625820042701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>1.1999999999999999E-14</v>
+      </c>
+      <c r="B7" s="1">
+        <v>1.09730427128784E-11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1.1999999999999999E-14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1.37853888960695E-11</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.1999999999999999E-14</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1.43467811595155E-11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.1999999999999999E-14</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1.8750405436853398E-11</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1.1999999999999999E-14</v>
+      </c>
+      <c r="J7" s="1">
+        <v>1.3930196176145199E-11</v>
+      </c>
+      <c r="K7" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="L7" s="1">
+        <v>16.048937659543</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1.4999999999999999E-14</v>
+      </c>
+      <c r="B8" s="1">
+        <v>9.5252530997871801E-12</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.4999999999999999E-14</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.23318760920764E-11</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1.4999999999999999E-14</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1.3134065942708701E-11</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1.4999999999999999E-14</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.7460322586155099E-11</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1.4999999999999999E-14</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1.26114788181629E-11</v>
+      </c>
+      <c r="K8" s="1">
+        <v>11.1</v>
+      </c>
+      <c r="L8" s="1">
+        <v>14.9737094602475</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>2E-14</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.2354895619669506E-12</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2E-14</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.09965782399377E-11</v>
+      </c>
+      <c r="E9" s="1">
+        <v>2E-14</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.2027168886031101E-11</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2E-14</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.61772844351935E-11</v>
+      </c>
+      <c r="I9" s="1">
+        <v>2E-14</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.14199292404394E-11</v>
+      </c>
+      <c r="K9" s="1">
+        <v>14.2</v>
+      </c>
+      <c r="L9" s="1">
+        <v>12.8983322565335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>2.5000000000000001E-14</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7.5169787009641899E-12</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2.5000000000000001E-14</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1.0247521615418601E-11</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2.5000000000000001E-14</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.1354578019623E-11</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.5000000000000001E-14</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.5416993016005699E-11</v>
+      </c>
+      <c r="I10" s="1">
+        <v>2.5000000000000001E-14</v>
+      </c>
+      <c r="J10" s="1">
+        <v>1.0743955796934001E-11</v>
+      </c>
+      <c r="K10" s="1">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="L10" s="1">
+        <v>11.4799825783817</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.0635480107031296E-12</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="D11" s="1">
+        <v>9.7440156499132896E-12</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1.09129056644596E-11</v>
+      </c>
+      <c r="G11" s="1">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.4894080475975101E-11</v>
+      </c>
+      <c r="I11" s="1">
+        <v>2.9999999999999998E-14</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1.02645851427967E-11</v>
+      </c>
+      <c r="K11" s="1">
+        <v>28.2</v>
+      </c>
+      <c r="L11">
+        <v>11.415248573725799</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>